<commit_message>
A new data sheet named CALCULATION added to the existing spread sheet which contains some mathematical calculation regarding data analysis
</commit_message>
<xml_diff>
--- a/Excel file Analysis/beginner-DA-course-blank.xlsx
+++ b/Excel file Analysis/beginner-DA-course-blank.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Chandoo.org\Formulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\Local Repo\Machine Learning\Excel file Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D2694-286C-4A36-ABB6-670D266C642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE6A06C-FB52-4827-B4BC-C04B19791C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{26D4546B-D2A1-4444-8EAF-A6228F96F0C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculation" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$C$11:$G$11</definedName>
@@ -36,8 +37,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Benajir Shuvo</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{68858B2F-84A7-431A-9E4A-D4BCB309DBA5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benajir Shuvo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Median is the mid point of a column arranged in a sorted way</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{3C6D835E-54A3-4B9E-B343-DEA1528CE378}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Benajir Shuvo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+First Quartile refers to the 1/4th points in your data when it is arranged in sort order</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="63">
   <si>
     <t>Product</t>
   </si>
@@ -206,16 +265,37 @@
   <si>
     <t>Are there any anomalies in the data?</t>
   </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>First Q</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +316,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -288,7 +381,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -297,14 +390,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,9 +447,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>2314878</xdr:colOff>
+      <xdr:colOff>2311703</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -433,7 +550,20 @@
   <autoFilter ref="Y11:Z33" xr:uid="{6DAC1E92-D947-4232-891E-65555AD7A47E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B8963D1-E60F-4400-A175-651A513B826F}" name="Product"/>
-    <tableColumn id="2" xr3:uid="{1798A7DA-FB9F-46D3-AA0A-B6BCA4A81AC3}" name="Cost per unit" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{1798A7DA-FB9F-46D3-AA0A-B6BCA4A81AC3}" name="Cost per unit" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{776EC52B-22F7-4298-9BE8-54AA728BCE4E}" name="data" displayName="data" ref="C11:G311" totalsRowShown="0" headerRowDxfId="0">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2A31AC7B-67A0-4CD5-AB3C-5CC0FD2A4B2C}" name="Sales Person"/>
+    <tableColumn id="2" xr3:uid="{8ED73118-6566-490C-B3C4-AAE707A3210E}" name="Geography"/>
+    <tableColumn id="3" xr3:uid="{6FC419BB-947D-419D-AD73-105B4D5FD2E6}" name="Product"/>
+    <tableColumn id="4" xr3:uid="{04091F2C-79AF-472B-9E70-5D01ADE3C55B}" name="Amount" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9917C258-D00A-4A7E-8C41-6A740AE146AE}" name="Units" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -738,33 +868,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE182796-6443-4558-9B87-909B73329DFC}">
   <dimension ref="A1:Z658"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" customWidth="1"/>
-    <col min="11" max="11" width="53.85546875" customWidth="1"/>
-    <col min="25" max="25" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" customWidth="1"/>
-    <col min="31" max="31" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" customWidth="1"/>
+    <col min="2" max="2" width="3.7265625" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="10" max="10" width="3.81640625" customWidth="1"/>
+    <col min="11" max="11" width="53.81640625" customWidth="1"/>
+    <col min="25" max="25" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.453125" customWidth="1"/>
+    <col min="31" max="31" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
@@ -791,7 +921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>40</v>
       </c>
@@ -820,7 +950,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>8</v>
       </c>
@@ -849,7 +979,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -878,7 +1008,7 @@
         <v>11.88</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>41</v>
       </c>
@@ -907,7 +1037,7 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>6</v>
       </c>
@@ -936,7 +1066,7 @@
         <v>8.7899999999999991</v>
       </c>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>40</v>
       </c>
@@ -965,7 +1095,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>6</v>
       </c>
@@ -994,7 +1124,7 @@
         <v>6.47</v>
       </c>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1153,7 @@
         <v>7.64</v>
       </c>
     </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1182,7 @@
         <v>10.62</v>
       </c>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>5</v>
       </c>
@@ -1081,7 +1211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>2</v>
       </c>
@@ -1104,7 +1234,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>3</v>
       </c>
@@ -1127,7 +1257,7 @@
         <v>6.49</v>
       </c>
     </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1280,7 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>2</v>
       </c>
@@ -1173,7 +1303,7 @@
         <v>13.15</v>
       </c>
     </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1326,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1349,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>6</v>
       </c>
@@ -1242,7 +1372,7 @@
         <v>10.38</v>
       </c>
     </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C29" t="s">
         <v>5</v>
       </c>
@@ -1265,7 +1395,7 @@
         <v>7.16</v>
       </c>
     </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
         <v>41</v>
       </c>
@@ -1288,7 +1418,7 @@
         <v>14.49</v>
       </c>
     </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>2</v>
       </c>
@@ -1311,7 +1441,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>9</v>
       </c>
@@ -1334,7 +1464,7 @@
         <v>8.65</v>
       </c>
     </row>
-    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>8</v>
       </c>
@@ -1357,7 +1487,7 @@
         <v>12.37</v>
       </c>
     </row>
-    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>10</v>
       </c>
@@ -1374,7 +1504,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +1521,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>41</v>
       </c>
@@ -1408,7 +1538,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
         <v>41</v>
       </c>
@@ -1425,7 +1555,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>3</v>
       </c>
@@ -1442,7 +1572,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>10</v>
       </c>
@@ -1459,7 +1589,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>5</v>
       </c>
@@ -1476,7 +1606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>10</v>
       </c>
@@ -1493,7 +1623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
         <v>41</v>
       </c>
@@ -1510,7 +1640,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>2</v>
       </c>
@@ -1527,7 +1657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
         <v>8</v>
       </c>
@@ -1544,7 +1674,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>40</v>
       </c>
@@ -1561,7 +1691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
         <v>41</v>
       </c>
@@ -1578,7 +1708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>6</v>
       </c>
@@ -1595,7 +1725,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:26" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
         <v>2</v>
       </c>
@@ -1612,7 +1742,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
         <v>6</v>
       </c>
@@ -1629,7 +1759,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1776,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
         <v>40</v>
       </c>
@@ -1663,7 +1793,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" t="s">
         <v>5</v>
       </c>
@@ -1680,7 +1810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" t="s">
         <v>2</v>
       </c>
@@ -1697,7 +1827,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1861,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" t="s">
         <v>2</v>
       </c>
@@ -1748,7 +1878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
         <v>6</v>
       </c>
@@ -1765,7 +1895,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>5</v>
       </c>
@@ -1782,7 +1912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" t="s">
         <v>3</v>
       </c>
@@ -1799,7 +1929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
         <v>6</v>
       </c>
@@ -1816,7 +1946,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" t="s">
         <v>40</v>
       </c>
@@ -1833,7 +1963,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
         <v>5</v>
       </c>
@@ -1850,7 +1980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" t="s">
         <v>6</v>
       </c>
@@ -1867,7 +1997,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" t="s">
         <v>2</v>
       </c>
@@ -1884,7 +2014,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" t="s">
         <v>2</v>
       </c>
@@ -1901,7 +2031,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" t="s">
         <v>41</v>
       </c>
@@ -1918,7 +2048,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" t="s">
         <v>40</v>
       </c>
@@ -1935,7 +2065,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" t="s">
         <v>41</v>
       </c>
@@ -1952,7 +2082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" t="s">
         <v>3</v>
       </c>
@@ -1969,7 +2099,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" t="s">
         <v>9</v>
       </c>
@@ -1986,7 +2116,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" t="s">
         <v>5</v>
       </c>
@@ -2003,7 +2133,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
         <v>6</v>
       </c>
@@ -2020,7 +2150,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" t="s">
         <v>6</v>
       </c>
@@ -2037,7 +2167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" t="s">
         <v>10</v>
       </c>
@@ -2054,7 +2184,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" t="s">
         <v>6</v>
       </c>
@@ -2071,7 +2201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" t="s">
         <v>8</v>
       </c>
@@ -2088,7 +2218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" t="s">
         <v>7</v>
       </c>
@@ -2105,7 +2235,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" t="s">
         <v>7</v>
       </c>
@@ -2122,7 +2252,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" t="s">
         <v>5</v>
       </c>
@@ -2139,7 +2269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" t="s">
         <v>40</v>
       </c>
@@ -2156,7 +2286,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C81" t="s">
         <v>5</v>
       </c>
@@ -2173,7 +2303,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C82" t="s">
         <v>10</v>
       </c>
@@ -2190,7 +2320,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C83" t="s">
         <v>7</v>
       </c>
@@ -2207,7 +2337,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C84" t="s">
         <v>9</v>
       </c>
@@ -2224,7 +2354,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C85" t="s">
         <v>9</v>
       </c>
@@ -2241,7 +2371,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C86" t="s">
         <v>5</v>
       </c>
@@ -2258,7 +2388,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C87" t="s">
         <v>3</v>
       </c>
@@ -2275,7 +2405,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C88" t="s">
         <v>41</v>
       </c>
@@ -2292,7 +2422,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C89" t="s">
         <v>6</v>
       </c>
@@ -2309,7 +2439,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C90" t="s">
         <v>9</v>
       </c>
@@ -2326,7 +2456,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C91" t="s">
         <v>5</v>
       </c>
@@ -2343,7 +2473,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C92" t="s">
         <v>8</v>
       </c>
@@ -2360,7 +2490,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C93" t="s">
         <v>2</v>
       </c>
@@ -2377,7 +2507,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C94" t="s">
         <v>3</v>
       </c>
@@ -2394,7 +2524,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C95" t="s">
         <v>10</v>
       </c>
@@ -2411,7 +2541,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C96" t="s">
         <v>10</v>
       </c>
@@ -2428,7 +2558,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C97" t="s">
         <v>2</v>
       </c>
@@ -2445,7 +2575,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
         <v>40</v>
       </c>
@@ -2462,7 +2592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
         <v>3</v>
       </c>
@@ -2479,7 +2609,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>10</v>
       </c>
@@ -2496,7 +2626,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>10</v>
       </c>
@@ -2513,7 +2643,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
         <v>5</v>
       </c>
@@ -2530,7 +2660,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
         <v>41</v>
       </c>
@@ -2547,7 +2677,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>3</v>
       </c>
@@ -2564,7 +2694,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>6</v>
       </c>
@@ -2581,7 +2711,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>9</v>
       </c>
@@ -2598,7 +2728,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>9</v>
       </c>
@@ -2615,7 +2745,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>9</v>
       </c>
@@ -2632,7 +2762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>3</v>
       </c>
@@ -2649,7 +2779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>40</v>
       </c>
@@ -2666,7 +2796,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
         <v>3</v>
       </c>
@@ -2683,7 +2813,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
         <v>7</v>
       </c>
@@ -2700,7 +2830,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C113" t="s">
         <v>2</v>
       </c>
@@ -2717,7 +2847,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C114" t="s">
         <v>41</v>
       </c>
@@ -2734,7 +2864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
         <v>5</v>
       </c>
@@ -2751,7 +2881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
         <v>40</v>
       </c>
@@ -2768,7 +2898,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
         <v>7</v>
       </c>
@@ -2785,7 +2915,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="118" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C118" t="s">
         <v>2</v>
       </c>
@@ -2802,7 +2932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C119" t="s">
         <v>40</v>
       </c>
@@ -2819,7 +2949,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
         <v>10</v>
       </c>
@@ -2836,7 +2966,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
         <v>8</v>
       </c>
@@ -2853,7 +2983,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C122" t="s">
         <v>5</v>
       </c>
@@ -2870,7 +3000,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="123" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C123" t="s">
         <v>41</v>
       </c>
@@ -2887,7 +3017,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="124" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
         <v>7</v>
       </c>
@@ -2904,7 +3034,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="125" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C125" t="s">
         <v>6</v>
       </c>
@@ -2921,7 +3051,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="126" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
         <v>10</v>
       </c>
@@ -2938,7 +3068,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C127" t="s">
         <v>6</v>
       </c>
@@ -2955,7 +3085,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C128" t="s">
         <v>6</v>
       </c>
@@ -2972,7 +3102,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C129" t="s">
         <v>7</v>
       </c>
@@ -2989,7 +3119,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C130" t="s">
         <v>2</v>
       </c>
@@ -3006,7 +3136,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C131" t="s">
         <v>40</v>
       </c>
@@ -3023,7 +3153,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C132" t="s">
         <v>41</v>
       </c>
@@ -3040,7 +3170,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C133" t="s">
         <v>40</v>
       </c>
@@ -3057,7 +3187,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C134" t="s">
         <v>41</v>
       </c>
@@ -3074,7 +3204,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C135" t="s">
         <v>8</v>
       </c>
@@ -3091,7 +3221,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="136" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C136" t="s">
         <v>6</v>
       </c>
@@ -3108,7 +3238,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C137" t="s">
         <v>7</v>
       </c>
@@ -3125,7 +3255,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C138" t="s">
         <v>7</v>
       </c>
@@ -3142,7 +3272,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C139" t="s">
         <v>7</v>
       </c>
@@ -3159,7 +3289,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C140" t="s">
         <v>10</v>
       </c>
@@ -3176,7 +3306,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C141" t="s">
         <v>7</v>
       </c>
@@ -3193,7 +3323,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="142" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C142" t="s">
         <v>8</v>
       </c>
@@ -3210,7 +3340,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C143" t="s">
         <v>7</v>
       </c>
@@ -3227,7 +3357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C144" t="s">
         <v>5</v>
       </c>
@@ -3244,7 +3374,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C145" t="s">
         <v>7</v>
       </c>
@@ -3261,7 +3391,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C146" t="s">
         <v>5</v>
       </c>
@@ -3278,7 +3408,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C147" t="s">
         <v>7</v>
       </c>
@@ -3295,7 +3425,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C148" t="s">
         <v>6</v>
       </c>
@@ -3312,7 +3442,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="149" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C149" t="s">
         <v>8</v>
       </c>
@@ -3329,7 +3459,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C150" t="s">
         <v>5</v>
       </c>
@@ -3346,7 +3476,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C151" t="s">
         <v>9</v>
       </c>
@@ -3363,7 +3493,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="152" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C152" t="s">
         <v>8</v>
       </c>
@@ -3380,7 +3510,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C153" t="s">
         <v>41</v>
       </c>
@@ -3397,7 +3527,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C154" t="s">
         <v>7</v>
       </c>
@@ -3414,7 +3544,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C155" t="s">
         <v>41</v>
       </c>
@@ -3431,7 +3561,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C156" t="s">
         <v>2</v>
       </c>
@@ -3448,7 +3578,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C157" t="s">
         <v>8</v>
       </c>
@@ -3465,7 +3595,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="158" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C158" t="s">
         <v>6</v>
       </c>
@@ -3482,7 +3612,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C159" t="s">
         <v>9</v>
       </c>
@@ -3499,7 +3629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C160" t="s">
         <v>2</v>
       </c>
@@ -3516,7 +3646,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C161" t="s">
         <v>6</v>
       </c>
@@ -3533,7 +3663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C162" t="s">
         <v>8</v>
       </c>
@@ -3550,7 +3680,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C163" t="s">
         <v>9</v>
       </c>
@@ -3567,7 +3697,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C164" t="s">
         <v>7</v>
       </c>
@@ -3584,7 +3714,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C165" t="s">
         <v>40</v>
       </c>
@@ -3601,7 +3731,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C166" t="s">
         <v>7</v>
       </c>
@@ -3618,7 +3748,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C167" t="s">
         <v>6</v>
       </c>
@@ -3635,7 +3765,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C168" t="s">
         <v>5</v>
       </c>
@@ -3652,7 +3782,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="169" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C169" t="s">
         <v>6</v>
       </c>
@@ -3669,7 +3799,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="170" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C170" t="s">
         <v>3</v>
       </c>
@@ -3686,7 +3816,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C171" t="s">
         <v>9</v>
       </c>
@@ -3703,7 +3833,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C172" t="s">
         <v>2</v>
       </c>
@@ -3720,7 +3850,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C173" t="s">
         <v>40</v>
       </c>
@@ -3737,7 +3867,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C174" t="s">
         <v>40</v>
       </c>
@@ -3754,7 +3884,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C175" t="s">
         <v>7</v>
       </c>
@@ -3771,7 +3901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C176" t="s">
         <v>40</v>
       </c>
@@ -3788,7 +3918,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C177" t="s">
         <v>10</v>
       </c>
@@ -3805,7 +3935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C178" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +3952,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C179" t="s">
         <v>40</v>
       </c>
@@ -3839,7 +3969,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="180" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C180" t="s">
         <v>3</v>
       </c>
@@ -3856,7 +3986,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="181" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C181" t="s">
         <v>3</v>
       </c>
@@ -3873,7 +4003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C182" t="s">
         <v>7</v>
       </c>
@@ -3890,7 +4020,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C183" t="s">
         <v>5</v>
       </c>
@@ -3907,7 +4037,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="184" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C184" t="s">
         <v>10</v>
       </c>
@@ -3924,7 +4054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C185" t="s">
         <v>8</v>
       </c>
@@ -3941,7 +4071,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C186" t="s">
         <v>2</v>
       </c>
@@ -3958,7 +4088,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="187" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C187" t="s">
         <v>41</v>
       </c>
@@ -3975,7 +4105,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="188" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C188" t="s">
         <v>40</v>
       </c>
@@ -3992,7 +4122,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C189" t="s">
         <v>6</v>
       </c>
@@ -4009,7 +4139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="190" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C190" t="s">
         <v>8</v>
       </c>
@@ -4026,7 +4156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C191" t="s">
         <v>9</v>
       </c>
@@ -4043,7 +4173,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C192" t="s">
         <v>6</v>
       </c>
@@ -4060,7 +4190,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="193" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C193" t="s">
         <v>10</v>
       </c>
@@ -4077,7 +4207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="194" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C194" t="s">
         <v>41</v>
       </c>
@@ -4094,7 +4224,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="195" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C195" t="s">
         <v>3</v>
       </c>
@@ -4111,7 +4241,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C196" t="s">
         <v>10</v>
       </c>
@@ -4128,7 +4258,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="197" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C197" t="s">
         <v>3</v>
       </c>
@@ -4145,7 +4275,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="198" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C198" t="s">
         <v>8</v>
       </c>
@@ -4162,7 +4292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="199" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C199" t="s">
         <v>40</v>
       </c>
@@ -4179,7 +4309,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="200" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C200" t="s">
         <v>6</v>
       </c>
@@ -4196,7 +4326,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="201" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C201" t="s">
         <v>5</v>
       </c>
@@ -4213,7 +4343,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="202" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C202" t="s">
         <v>9</v>
       </c>
@@ -4230,7 +4360,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="203" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C203" t="s">
         <v>8</v>
       </c>
@@ -4247,7 +4377,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C204" t="s">
         <v>7</v>
       </c>
@@ -4264,7 +4394,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="205" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C205" t="s">
         <v>3</v>
       </c>
@@ -4281,7 +4411,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="206" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C206" t="s">
         <v>6</v>
       </c>
@@ -4298,7 +4428,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="207" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C207" t="s">
         <v>9</v>
       </c>
@@ -4315,7 +4445,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="208" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C208" t="s">
         <v>9</v>
       </c>
@@ -4332,7 +4462,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="209" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C209" t="s">
         <v>8</v>
       </c>
@@ -4349,7 +4479,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="210" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C210" t="s">
         <v>40</v>
       </c>
@@ -4366,7 +4496,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="211" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C211" t="s">
         <v>40</v>
       </c>
@@ -4383,7 +4513,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="212" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C212" t="s">
         <v>41</v>
       </c>
@@ -4400,7 +4530,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="213" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C213" t="s">
         <v>41</v>
       </c>
@@ -4417,7 +4547,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="214" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C214" t="s">
         <v>5</v>
       </c>
@@ -4434,7 +4564,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="215" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C215" t="s">
         <v>40</v>
       </c>
@@ -4451,7 +4581,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="216" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C216" t="s">
         <v>2</v>
       </c>
@@ -4468,7 +4598,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="217" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C217" t="s">
         <v>7</v>
       </c>
@@ -4485,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C218" t="s">
         <v>5</v>
       </c>
@@ -4502,7 +4632,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="219" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C219" t="s">
         <v>9</v>
       </c>
@@ -4519,7 +4649,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="220" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C220" t="s">
         <v>7</v>
       </c>
@@ -4536,7 +4666,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="221" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C221" t="s">
         <v>6</v>
       </c>
@@ -4553,7 +4683,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="222" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C222" t="s">
         <v>41</v>
       </c>
@@ -4570,7 +4700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="223" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C223" t="s">
         <v>7</v>
       </c>
@@ -4587,7 +4717,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="224" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C224" t="s">
         <v>9</v>
       </c>
@@ -4604,7 +4734,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="225" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C225" t="s">
         <v>5</v>
       </c>
@@ -4621,7 +4751,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="226" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C226" t="s">
         <v>9</v>
       </c>
@@ -4638,7 +4768,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="227" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C227" t="s">
         <v>10</v>
       </c>
@@ -4655,7 +4785,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="228" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C228" t="s">
         <v>2</v>
       </c>
@@ -4672,7 +4802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C229" t="s">
         <v>7</v>
       </c>
@@ -4689,7 +4819,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="230" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C230" t="s">
         <v>5</v>
       </c>
@@ -4706,7 +4836,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="231" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C231" t="s">
         <v>6</v>
       </c>
@@ -4723,7 +4853,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="232" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C232" t="s">
         <v>9</v>
       </c>
@@ -4740,7 +4870,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="233" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C233" t="s">
         <v>7</v>
       </c>
@@ -4757,7 +4887,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="234" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C234" t="s">
         <v>41</v>
       </c>
@@ -4774,7 +4904,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="235" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C235" t="s">
         <v>2</v>
       </c>
@@ -4791,7 +4921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="236" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C236" t="s">
         <v>9</v>
       </c>
@@ -4808,7 +4938,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="237" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C237" t="s">
         <v>3</v>
       </c>
@@ -4825,7 +4955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="238" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C238" t="s">
         <v>9</v>
       </c>
@@ -4842,7 +4972,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="239" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C239" t="s">
         <v>9</v>
       </c>
@@ -4859,7 +4989,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C240" t="s">
         <v>41</v>
       </c>
@@ -4876,7 +5006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C241" t="s">
         <v>10</v>
       </c>
@@ -4893,7 +5023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="242" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C242" t="s">
         <v>5</v>
       </c>
@@ -4910,7 +5040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="243" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C243" t="s">
         <v>5</v>
       </c>
@@ -4927,7 +5057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C244" t="s">
         <v>8</v>
       </c>
@@ -4944,7 +5074,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="245" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C245" t="s">
         <v>6</v>
       </c>
@@ -4961,7 +5091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="246" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C246" t="s">
         <v>40</v>
       </c>
@@ -4978,7 +5108,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="247" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C247" t="s">
         <v>40</v>
       </c>
@@ -4995,7 +5125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="248" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C248" t="s">
         <v>5</v>
       </c>
@@ -5012,7 +5142,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="249" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C249" t="s">
         <v>40</v>
       </c>
@@ -5029,7 +5159,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="250" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C250" t="s">
         <v>6</v>
       </c>
@@ -5046,7 +5176,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="251" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C251" t="s">
         <v>3</v>
       </c>
@@ -5063,7 +5193,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="252" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C252" t="s">
         <v>40</v>
       </c>
@@ -5080,7 +5210,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="253" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C253" t="s">
         <v>10</v>
       </c>
@@ -5097,7 +5227,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="254" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C254" t="s">
         <v>8</v>
       </c>
@@ -5114,7 +5244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="255" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C255" t="s">
         <v>9</v>
       </c>
@@ -5131,7 +5261,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="256" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C256" t="s">
         <v>9</v>
       </c>
@@ -5148,7 +5278,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="257" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C257" t="s">
         <v>10</v>
       </c>
@@ -5165,7 +5295,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="258" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C258" t="s">
         <v>8</v>
       </c>
@@ -5182,7 +5312,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="259" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C259" t="s">
         <v>10</v>
       </c>
@@ -5199,7 +5329,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="260" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C260" t="s">
         <v>6</v>
       </c>
@@ -5216,7 +5346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="261" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C261" t="s">
         <v>2</v>
       </c>
@@ -5233,7 +5363,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="262" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C262" t="s">
         <v>7</v>
       </c>
@@ -5250,7 +5380,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="263" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C263" t="s">
         <v>10</v>
       </c>
@@ -5267,7 +5397,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="264" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C264" t="s">
         <v>40</v>
       </c>
@@ -5284,7 +5414,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="265" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C265" t="s">
         <v>6</v>
       </c>
@@ -5301,7 +5431,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="266" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C266" t="s">
         <v>40</v>
       </c>
@@ -5318,7 +5448,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="267" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C267" t="s">
         <v>5</v>
       </c>
@@ -5335,7 +5465,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="268" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C268" t="s">
         <v>40</v>
       </c>
@@ -5352,7 +5482,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="269" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C269" t="s">
         <v>2</v>
       </c>
@@ -5369,7 +5499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="270" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C270" t="s">
         <v>5</v>
       </c>
@@ -5386,7 +5516,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="271" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C271" t="s">
         <v>8</v>
       </c>
@@ -5403,7 +5533,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="272" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C272" t="s">
         <v>7</v>
       </c>
@@ -5420,7 +5550,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="273" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C273" t="s">
         <v>3</v>
       </c>
@@ -5437,7 +5567,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="274" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C274" t="s">
         <v>8</v>
       </c>
@@ -5454,7 +5584,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="275" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C275" t="s">
         <v>3</v>
       </c>
@@ -5471,7 +5601,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="276" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C276" t="s">
         <v>41</v>
       </c>
@@ -5488,7 +5618,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="277" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C277" t="s">
         <v>40</v>
       </c>
@@ -5505,7 +5635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="278" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C278" t="s">
         <v>7</v>
       </c>
@@ -5522,7 +5652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="279" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C279" t="s">
         <v>40</v>
       </c>
@@ -5539,7 +5669,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="280" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C280" t="s">
         <v>6</v>
       </c>
@@ -5556,7 +5686,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="281" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C281" t="s">
         <v>8</v>
       </c>
@@ -5573,7 +5703,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="282" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C282" t="s">
         <v>2</v>
       </c>
@@ -5590,7 +5720,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="283" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C283" t="s">
         <v>40</v>
       </c>
@@ -5607,7 +5737,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="284" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C284" t="s">
         <v>6</v>
       </c>
@@ -5624,7 +5754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="285" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C285" t="s">
         <v>3</v>
       </c>
@@ -5641,7 +5771,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="286" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C286" t="s">
         <v>3</v>
       </c>
@@ -5658,7 +5788,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="287" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C287" t="s">
         <v>2</v>
       </c>
@@ -5675,7 +5805,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="288" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C288" t="s">
         <v>6</v>
       </c>
@@ -5692,7 +5822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C289" t="s">
         <v>8</v>
       </c>
@@ -5709,7 +5839,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="290" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C290" t="s">
         <v>5</v>
       </c>
@@ -5726,7 +5856,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="291" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C291" t="s">
         <v>2</v>
       </c>
@@ -5743,7 +5873,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="292" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C292" t="s">
         <v>2</v>
       </c>
@@ -5760,7 +5890,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="293" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C293" t="s">
         <v>41</v>
       </c>
@@ -5777,7 +5907,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="294" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C294" t="s">
         <v>6</v>
       </c>
@@ -5794,7 +5924,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="295" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C295" t="s">
         <v>5</v>
       </c>
@@ -5811,7 +5941,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="296" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C296" t="s">
         <v>10</v>
       </c>
@@ -5828,7 +5958,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="297" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C297" t="s">
         <v>40</v>
       </c>
@@ -5845,7 +5975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="298" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C298" t="s">
         <v>6</v>
       </c>
@@ -5862,7 +5992,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="299" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C299" t="s">
         <v>10</v>
       </c>
@@ -5879,7 +6009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="300" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C300" t="s">
         <v>7</v>
       </c>
@@ -5896,7 +6026,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="301" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C301" t="s">
         <v>3</v>
       </c>
@@ -5913,7 +6043,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="302" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C302" t="s">
         <v>2</v>
       </c>
@@ -5930,7 +6060,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="303" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C303" t="s">
         <v>9</v>
       </c>
@@ -5947,7 +6077,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="304" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C304" t="s">
         <v>9</v>
       </c>
@@ -5964,7 +6094,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="305" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C305" t="s">
         <v>7</v>
       </c>
@@ -5981,7 +6111,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="306" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C306" t="s">
         <v>7</v>
       </c>
@@ -5998,7 +6128,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="307" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C307" t="s">
         <v>3</v>
       </c>
@@ -6015,7 +6145,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="308" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C308" t="s">
         <v>3</v>
       </c>
@@ -6032,7 +6162,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="309" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C309" t="s">
         <v>2</v>
       </c>
@@ -6049,7 +6179,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="310" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C310" t="s">
         <v>41</v>
       </c>
@@ -6066,7 +6196,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="311" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C311" t="s">
         <v>9</v>
       </c>
@@ -6083,1399 +6213,1494 @@
         <v>102</v>
       </c>
     </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F312" s="4"/>
       <c r="G312" s="5"/>
     </row>
-    <row r="313" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F313" s="4"/>
       <c r="G313" s="5"/>
     </row>
-    <row r="314" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F314" s="4"/>
       <c r="G314" s="5"/>
     </row>
-    <row r="315" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F315" s="4"/>
       <c r="G315" s="5"/>
     </row>
-    <row r="316" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F316" s="4"/>
       <c r="G316" s="5"/>
     </row>
-    <row r="317" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F317" s="4"/>
       <c r="G317" s="5"/>
     </row>
-    <row r="318" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F318" s="4"/>
       <c r="G318" s="5"/>
     </row>
-    <row r="319" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F319" s="4"/>
       <c r="G319" s="5"/>
     </row>
-    <row r="320" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:7" x14ac:dyDescent="0.35">
       <c r="F320" s="4"/>
       <c r="G320" s="5"/>
     </row>
-    <row r="321" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="321" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F321" s="4"/>
       <c r="G321" s="5"/>
     </row>
-    <row r="322" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="322" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F322" s="4"/>
       <c r="G322" s="5"/>
     </row>
-    <row r="323" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F323" s="4"/>
       <c r="G323" s="5"/>
     </row>
-    <row r="324" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F324" s="4"/>
       <c r="G324" s="5"/>
     </row>
-    <row r="325" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F325" s="4"/>
       <c r="G325" s="5"/>
     </row>
-    <row r="326" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="326" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F326" s="4"/>
       <c r="G326" s="5"/>
     </row>
-    <row r="327" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="327" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F327" s="4"/>
       <c r="G327" s="5"/>
     </row>
-    <row r="328" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="328" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F328" s="4"/>
       <c r="G328" s="5"/>
     </row>
-    <row r="329" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="329" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F329" s="4"/>
       <c r="G329" s="5"/>
     </row>
-    <row r="330" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="330" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F330" s="4"/>
       <c r="G330" s="5"/>
     </row>
-    <row r="331" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="331" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F331" s="4"/>
       <c r="G331" s="5"/>
     </row>
-    <row r="332" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="332" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F332" s="4"/>
       <c r="G332" s="5"/>
     </row>
-    <row r="333" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="333" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F333" s="4"/>
       <c r="G333" s="5"/>
     </row>
-    <row r="334" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="334" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F334" s="4"/>
       <c r="G334" s="5"/>
     </row>
-    <row r="335" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="335" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F335" s="4"/>
       <c r="G335" s="5"/>
     </row>
-    <row r="336" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="336" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F336" s="4"/>
       <c r="G336" s="5"/>
     </row>
-    <row r="337" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="337" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F337" s="4"/>
       <c r="G337" s="5"/>
     </row>
-    <row r="338" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="338" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F338" s="4"/>
       <c r="G338" s="5"/>
     </row>
-    <row r="339" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="339" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F339" s="4"/>
       <c r="G339" s="5"/>
     </row>
-    <row r="340" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="340" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F340" s="4"/>
       <c r="G340" s="5"/>
     </row>
-    <row r="341" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="341" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F341" s="4"/>
       <c r="G341" s="5"/>
     </row>
-    <row r="342" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="342" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F342" s="4"/>
       <c r="G342" s="5"/>
     </row>
-    <row r="343" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="343" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F343" s="4"/>
       <c r="G343" s="5"/>
     </row>
-    <row r="344" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="344" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F344" s="4"/>
       <c r="G344" s="5"/>
     </row>
-    <row r="345" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="345" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F345" s="4"/>
       <c r="G345" s="5"/>
     </row>
-    <row r="346" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="346" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F346" s="4"/>
       <c r="G346" s="5"/>
     </row>
-    <row r="347" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="347" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F347" s="4"/>
       <c r="G347" s="5"/>
     </row>
-    <row r="348" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="348" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F348" s="4"/>
       <c r="G348" s="5"/>
     </row>
-    <row r="349" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="349" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F349" s="4"/>
       <c r="G349" s="5"/>
     </row>
-    <row r="350" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="350" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F350" s="4"/>
       <c r="G350" s="5"/>
     </row>
-    <row r="351" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="351" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F351" s="4"/>
       <c r="G351" s="5"/>
     </row>
-    <row r="352" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="352" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F352" s="4"/>
       <c r="G352" s="5"/>
     </row>
-    <row r="353" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="353" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F353" s="4"/>
       <c r="G353" s="5"/>
     </row>
-    <row r="354" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F354" s="4"/>
       <c r="G354" s="5"/>
     </row>
-    <row r="355" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="355" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F355" s="4"/>
       <c r="G355" s="5"/>
     </row>
-    <row r="356" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="356" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F356" s="4"/>
       <c r="G356" s="5"/>
     </row>
-    <row r="357" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F357" s="4"/>
       <c r="G357" s="5"/>
     </row>
-    <row r="358" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="358" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F358" s="4"/>
       <c r="G358" s="5"/>
     </row>
-    <row r="359" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="359" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F359" s="4"/>
       <c r="G359" s="5"/>
     </row>
-    <row r="360" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="360" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F360" s="4"/>
       <c r="G360" s="5"/>
     </row>
-    <row r="361" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F361" s="4"/>
       <c r="G361" s="5"/>
     </row>
-    <row r="362" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="362" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F362" s="4"/>
       <c r="G362" s="5"/>
     </row>
-    <row r="363" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="363" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F363" s="4"/>
       <c r="G363" s="5"/>
     </row>
-    <row r="364" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="364" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F364" s="4"/>
       <c r="G364" s="5"/>
     </row>
-    <row r="365" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F365" s="4"/>
       <c r="G365" s="5"/>
     </row>
-    <row r="366" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="366" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F366" s="4"/>
       <c r="G366" s="5"/>
     </row>
-    <row r="367" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F367" s="4"/>
       <c r="G367" s="5"/>
     </row>
-    <row r="368" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="368" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F368" s="4"/>
       <c r="G368" s="5"/>
     </row>
-    <row r="369" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="369" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F369" s="4"/>
       <c r="G369" s="5"/>
     </row>
-    <row r="370" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F370" s="4"/>
       <c r="G370" s="5"/>
     </row>
-    <row r="371" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="371" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F371" s="4"/>
       <c r="G371" s="5"/>
     </row>
-    <row r="372" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="372" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F372" s="4"/>
       <c r="G372" s="5"/>
     </row>
-    <row r="373" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="373" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F373" s="4"/>
       <c r="G373" s="5"/>
     </row>
-    <row r="374" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="374" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F374" s="4"/>
       <c r="G374" s="5"/>
     </row>
-    <row r="375" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="375" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F375" s="4"/>
       <c r="G375" s="5"/>
     </row>
-    <row r="376" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="376" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F376" s="4"/>
       <c r="G376" s="5"/>
     </row>
-    <row r="377" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="377" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F377" s="4"/>
       <c r="G377" s="5"/>
     </row>
-    <row r="378" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="378" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F378" s="4"/>
       <c r="G378" s="5"/>
     </row>
-    <row r="379" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="379" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F379" s="4"/>
       <c r="G379" s="5"/>
     </row>
-    <row r="380" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="380" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F380" s="4"/>
       <c r="G380" s="5"/>
     </row>
-    <row r="381" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="381" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F381" s="4"/>
       <c r="G381" s="5"/>
     </row>
-    <row r="382" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="382" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F382" s="4"/>
       <c r="G382" s="5"/>
     </row>
-    <row r="383" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="383" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F383" s="4"/>
       <c r="G383" s="5"/>
     </row>
-    <row r="384" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="384" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F384" s="4"/>
       <c r="G384" s="5"/>
     </row>
-    <row r="385" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="385" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F385" s="4"/>
       <c r="G385" s="5"/>
     </row>
-    <row r="386" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="386" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F386" s="4"/>
       <c r="G386" s="5"/>
     </row>
-    <row r="387" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="387" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F387" s="4"/>
       <c r="G387" s="5"/>
     </row>
-    <row r="388" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="388" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F388" s="4"/>
       <c r="G388" s="5"/>
     </row>
-    <row r="389" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="389" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F389" s="4"/>
       <c r="G389" s="5"/>
     </row>
-    <row r="390" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="390" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F390" s="4"/>
       <c r="G390" s="5"/>
     </row>
-    <row r="391" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="391" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F391" s="4"/>
       <c r="G391" s="5"/>
     </row>
-    <row r="392" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="392" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F392" s="4"/>
       <c r="G392" s="5"/>
     </row>
-    <row r="393" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="393" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F393" s="4"/>
       <c r="G393" s="5"/>
     </row>
-    <row r="394" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="394" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F394" s="4"/>
       <c r="G394" s="5"/>
     </row>
-    <row r="395" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="395" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F395" s="4"/>
       <c r="G395" s="5"/>
     </row>
-    <row r="396" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="396" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F396" s="4"/>
       <c r="G396" s="5"/>
     </row>
-    <row r="397" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="397" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F397" s="4"/>
       <c r="G397" s="5"/>
     </row>
-    <row r="398" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="398" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F398" s="4"/>
       <c r="G398" s="5"/>
     </row>
-    <row r="399" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="399" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F399" s="4"/>
       <c r="G399" s="5"/>
     </row>
-    <row r="400" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="400" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F400" s="4"/>
       <c r="G400" s="5"/>
     </row>
-    <row r="401" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="401" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F401" s="4"/>
       <c r="G401" s="5"/>
     </row>
-    <row r="402" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="402" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F402" s="4"/>
       <c r="G402" s="5"/>
     </row>
-    <row r="403" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="403" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F403" s="4"/>
       <c r="G403" s="5"/>
     </row>
-    <row r="404" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="404" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F404" s="4"/>
       <c r="G404" s="5"/>
     </row>
-    <row r="405" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="405" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F405" s="4"/>
       <c r="G405" s="5"/>
     </row>
-    <row r="406" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="406" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F406" s="4"/>
       <c r="G406" s="5"/>
     </row>
-    <row r="407" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="407" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F407" s="4"/>
       <c r="G407" s="5"/>
     </row>
-    <row r="408" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="408" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F408" s="4"/>
       <c r="G408" s="5"/>
     </row>
-    <row r="409" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="409" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F409" s="4"/>
       <c r="G409" s="5"/>
     </row>
-    <row r="410" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="410" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F410" s="4"/>
       <c r="G410" s="5"/>
     </row>
-    <row r="411" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="411" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F411" s="4"/>
       <c r="G411" s="5"/>
     </row>
-    <row r="412" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="412" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F412" s="4"/>
       <c r="G412" s="5"/>
     </row>
-    <row r="413" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="413" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F413" s="4"/>
       <c r="G413" s="5"/>
     </row>
-    <row r="414" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="414" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F414" s="4"/>
       <c r="G414" s="5"/>
     </row>
-    <row r="415" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="415" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F415" s="4"/>
       <c r="G415" s="5"/>
     </row>
-    <row r="416" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="416" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F416" s="4"/>
       <c r="G416" s="5"/>
     </row>
-    <row r="417" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="417" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F417" s="4"/>
       <c r="G417" s="5"/>
     </row>
-    <row r="418" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="418" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F418" s="4"/>
       <c r="G418" s="5"/>
     </row>
-    <row r="419" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="419" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F419" s="4"/>
       <c r="G419" s="5"/>
     </row>
-    <row r="420" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="420" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F420" s="4"/>
       <c r="G420" s="5"/>
     </row>
-    <row r="421" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="421" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F421" s="4"/>
       <c r="G421" s="5"/>
     </row>
-    <row r="422" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="422" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F422" s="4"/>
       <c r="G422" s="5"/>
     </row>
-    <row r="423" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="423" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F423" s="4"/>
       <c r="G423" s="5"/>
     </row>
-    <row r="424" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="424" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F424" s="4"/>
       <c r="G424" s="5"/>
     </row>
-    <row r="425" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="425" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F425" s="4"/>
       <c r="G425" s="5"/>
     </row>
-    <row r="426" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="426" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F426" s="4"/>
       <c r="G426" s="5"/>
     </row>
-    <row r="427" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="427" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F427" s="4"/>
       <c r="G427" s="5"/>
     </row>
-    <row r="428" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="428" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F428" s="4"/>
       <c r="G428" s="5"/>
     </row>
-    <row r="429" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="429" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F429" s="4"/>
       <c r="G429" s="5"/>
     </row>
-    <row r="430" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="430" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F430" s="4"/>
       <c r="G430" s="5"/>
     </row>
-    <row r="431" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="431" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F431" s="4"/>
       <c r="G431" s="5"/>
     </row>
-    <row r="432" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="432" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F432" s="4"/>
       <c r="G432" s="5"/>
     </row>
-    <row r="433" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="433" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F433" s="4"/>
       <c r="G433" s="5"/>
     </row>
-    <row r="434" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="434" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F434" s="4"/>
       <c r="G434" s="5"/>
     </row>
-    <row r="435" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="435" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F435" s="4"/>
       <c r="G435" s="5"/>
     </row>
-    <row r="436" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="436" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F436" s="4"/>
       <c r="G436" s="5"/>
     </row>
-    <row r="437" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="437" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F437" s="4"/>
       <c r="G437" s="5"/>
     </row>
-    <row r="438" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="438" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F438" s="4"/>
       <c r="G438" s="5"/>
     </row>
-    <row r="439" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="439" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F439" s="4"/>
       <c r="G439" s="5"/>
     </row>
-    <row r="440" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="440" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F440" s="4"/>
       <c r="G440" s="5"/>
     </row>
-    <row r="441" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="441" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F441" s="4"/>
       <c r="G441" s="5"/>
     </row>
-    <row r="442" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="442" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F442" s="4"/>
       <c r="G442" s="5"/>
     </row>
-    <row r="443" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="443" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F443" s="4"/>
       <c r="G443" s="5"/>
     </row>
-    <row r="444" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="444" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F444" s="4"/>
       <c r="G444" s="5"/>
     </row>
-    <row r="445" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="445" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F445" s="4"/>
       <c r="G445" s="5"/>
     </row>
-    <row r="446" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="446" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F446" s="4"/>
       <c r="G446" s="5"/>
     </row>
-    <row r="447" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="447" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F447" s="4"/>
       <c r="G447" s="5"/>
     </row>
-    <row r="448" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="448" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F448" s="4"/>
       <c r="G448" s="5"/>
     </row>
-    <row r="449" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="449" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F449" s="4"/>
       <c r="G449" s="5"/>
     </row>
-    <row r="450" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="450" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F450" s="4"/>
       <c r="G450" s="5"/>
     </row>
-    <row r="451" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="451" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F451" s="4"/>
       <c r="G451" s="5"/>
     </row>
-    <row r="452" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="452" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F452" s="4"/>
       <c r="G452" s="5"/>
     </row>
-    <row r="453" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="453" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F453" s="4"/>
       <c r="G453" s="5"/>
     </row>
-    <row r="454" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="454" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F454" s="4"/>
       <c r="G454" s="5"/>
     </row>
-    <row r="455" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="455" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F455" s="4"/>
       <c r="G455" s="5"/>
     </row>
-    <row r="456" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="456" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F456" s="4"/>
       <c r="G456" s="5"/>
     </row>
-    <row r="457" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="457" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F457" s="4"/>
       <c r="G457" s="5"/>
     </row>
-    <row r="458" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="458" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F458" s="4"/>
       <c r="G458" s="5"/>
     </row>
-    <row r="459" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="459" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F459" s="4"/>
       <c r="G459" s="5"/>
     </row>
-    <row r="460" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="460" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F460" s="4"/>
       <c r="G460" s="5"/>
     </row>
-    <row r="461" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="461" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F461" s="4"/>
       <c r="G461" s="5"/>
     </row>
-    <row r="462" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="462" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F462" s="4"/>
       <c r="G462" s="5"/>
     </row>
-    <row r="463" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="463" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F463" s="4"/>
       <c r="G463" s="5"/>
     </row>
-    <row r="464" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="464" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F464" s="4"/>
       <c r="G464" s="5"/>
     </row>
-    <row r="465" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="465" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F465" s="4"/>
       <c r="G465" s="5"/>
     </row>
-    <row r="466" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="466" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F466" s="4"/>
       <c r="G466" s="5"/>
     </row>
-    <row r="467" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="467" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F467" s="4"/>
       <c r="G467" s="5"/>
     </row>
-    <row r="468" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="468" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F468" s="4"/>
       <c r="G468" s="5"/>
     </row>
-    <row r="469" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="469" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F469" s="4"/>
       <c r="G469" s="5"/>
     </row>
-    <row r="470" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="470" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F470" s="4"/>
       <c r="G470" s="5"/>
     </row>
-    <row r="471" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="471" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F471" s="4"/>
       <c r="G471" s="5"/>
     </row>
-    <row r="472" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="472" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F472" s="4"/>
       <c r="G472" s="5"/>
     </row>
-    <row r="473" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="473" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F473" s="4"/>
       <c r="G473" s="5"/>
     </row>
-    <row r="474" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="474" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F474" s="4"/>
       <c r="G474" s="5"/>
     </row>
-    <row r="475" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="475" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F475" s="4"/>
       <c r="G475" s="5"/>
     </row>
-    <row r="476" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="476" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F476" s="4"/>
       <c r="G476" s="5"/>
     </row>
-    <row r="477" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="477" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F477" s="4"/>
       <c r="G477" s="5"/>
     </row>
-    <row r="478" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="478" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F478" s="4"/>
       <c r="G478" s="5"/>
     </row>
-    <row r="479" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="479" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F479" s="4"/>
       <c r="G479" s="5"/>
     </row>
-    <row r="480" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="480" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F480" s="4"/>
       <c r="G480" s="5"/>
     </row>
-    <row r="481" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="481" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F481" s="4"/>
       <c r="G481" s="5"/>
     </row>
-    <row r="482" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="482" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F482" s="4"/>
       <c r="G482" s="5"/>
     </row>
-    <row r="483" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="483" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F483" s="4"/>
       <c r="G483" s="5"/>
     </row>
-    <row r="484" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="484" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F484" s="4"/>
       <c r="G484" s="5"/>
     </row>
-    <row r="485" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="485" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F485" s="4"/>
       <c r="G485" s="5"/>
     </row>
-    <row r="486" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="486" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F486" s="4"/>
       <c r="G486" s="5"/>
     </row>
-    <row r="487" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="487" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F487" s="4"/>
       <c r="G487" s="5"/>
     </row>
-    <row r="488" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="488" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F488" s="4"/>
       <c r="G488" s="5"/>
     </row>
-    <row r="489" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="489" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F489" s="4"/>
       <c r="G489" s="5"/>
     </row>
-    <row r="490" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="490" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F490" s="4"/>
       <c r="G490" s="5"/>
     </row>
-    <row r="491" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="491" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F491" s="4"/>
       <c r="G491" s="5"/>
     </row>
-    <row r="492" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="492" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F492" s="4"/>
       <c r="G492" s="5"/>
     </row>
-    <row r="493" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="493" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F493" s="4"/>
       <c r="G493" s="5"/>
     </row>
-    <row r="494" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="494" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F494" s="4"/>
       <c r="G494" s="5"/>
     </row>
-    <row r="495" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="495" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F495" s="4"/>
       <c r="G495" s="5"/>
     </row>
-    <row r="496" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="496" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F496" s="4"/>
       <c r="G496" s="5"/>
     </row>
-    <row r="497" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="497" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F497" s="4"/>
       <c r="G497" s="5"/>
     </row>
-    <row r="498" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="498" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F498" s="4"/>
       <c r="G498" s="5"/>
     </row>
-    <row r="499" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="499" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F499" s="4"/>
       <c r="G499" s="5"/>
     </row>
-    <row r="500" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="500" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F500" s="4"/>
       <c r="G500" s="5"/>
     </row>
-    <row r="501" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="501" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F501" s="4"/>
       <c r="G501" s="5"/>
     </row>
-    <row r="502" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="502" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F502" s="4"/>
       <c r="G502" s="5"/>
     </row>
-    <row r="503" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="503" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F503" s="4"/>
       <c r="G503" s="5"/>
     </row>
-    <row r="504" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="504" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F504" s="4"/>
       <c r="G504" s="5"/>
     </row>
-    <row r="505" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="505" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F505" s="4"/>
       <c r="G505" s="5"/>
     </row>
-    <row r="506" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="506" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F506" s="4"/>
       <c r="G506" s="5"/>
     </row>
-    <row r="507" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="507" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F507" s="4"/>
       <c r="G507" s="5"/>
     </row>
-    <row r="508" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="508" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F508" s="4"/>
       <c r="G508" s="5"/>
     </row>
-    <row r="509" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="509" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F509" s="4"/>
       <c r="G509" s="5"/>
     </row>
-    <row r="510" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="510" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F510" s="4"/>
       <c r="G510" s="5"/>
     </row>
-    <row r="511" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="511" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F511" s="4"/>
       <c r="G511" s="5"/>
     </row>
-    <row r="512" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="512" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F512" s="4"/>
       <c r="G512" s="5"/>
     </row>
-    <row r="513" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="513" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F513" s="4"/>
       <c r="G513" s="5"/>
     </row>
-    <row r="514" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="514" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F514" s="4"/>
       <c r="G514" s="5"/>
     </row>
-    <row r="515" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="515" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F515" s="4"/>
       <c r="G515" s="5"/>
     </row>
-    <row r="516" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="516" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F516" s="4"/>
       <c r="G516" s="5"/>
     </row>
-    <row r="517" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="517" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F517" s="4"/>
       <c r="G517" s="5"/>
     </row>
-    <row r="518" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="518" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F518" s="4"/>
       <c r="G518" s="5"/>
     </row>
-    <row r="519" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="519" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F519" s="4"/>
       <c r="G519" s="5"/>
     </row>
-    <row r="520" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="520" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F520" s="4"/>
       <c r="G520" s="5"/>
     </row>
-    <row r="521" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="521" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F521" s="4"/>
       <c r="G521" s="5"/>
     </row>
-    <row r="522" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="522" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F522" s="4"/>
       <c r="G522" s="5"/>
     </row>
-    <row r="523" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="523" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F523" s="4"/>
       <c r="G523" s="5"/>
     </row>
-    <row r="524" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="524" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F524" s="4"/>
       <c r="G524" s="5"/>
     </row>
-    <row r="525" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="525" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F525" s="4"/>
       <c r="G525" s="5"/>
     </row>
-    <row r="526" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="526" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F526" s="4"/>
       <c r="G526" s="5"/>
     </row>
-    <row r="527" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="527" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F527" s="4"/>
       <c r="G527" s="5"/>
     </row>
-    <row r="528" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="528" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F528" s="4"/>
       <c r="G528" s="5"/>
     </row>
-    <row r="529" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="529" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F529" s="4"/>
       <c r="G529" s="5"/>
     </row>
-    <row r="530" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="530" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F530" s="4"/>
       <c r="G530" s="5"/>
     </row>
-    <row r="531" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="531" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F531" s="4"/>
       <c r="G531" s="5"/>
     </row>
-    <row r="532" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="532" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F532" s="4"/>
       <c r="G532" s="5"/>
     </row>
-    <row r="533" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="533" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F533" s="4"/>
       <c r="G533" s="5"/>
     </row>
-    <row r="534" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="534" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F534" s="4"/>
       <c r="G534" s="5"/>
     </row>
-    <row r="535" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="535" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F535" s="4"/>
       <c r="G535" s="5"/>
     </row>
-    <row r="536" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="536" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F536" s="4"/>
       <c r="G536" s="5"/>
     </row>
-    <row r="537" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="537" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F537" s="4"/>
       <c r="G537" s="5"/>
     </row>
-    <row r="538" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="538" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F538" s="4"/>
       <c r="G538" s="5"/>
     </row>
-    <row r="539" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="539" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F539" s="4"/>
       <c r="G539" s="5"/>
     </row>
-    <row r="540" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="540" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F540" s="4"/>
       <c r="G540" s="5"/>
     </row>
-    <row r="541" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="541" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F541" s="4"/>
       <c r="G541" s="5"/>
     </row>
-    <row r="542" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="542" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F542" s="4"/>
       <c r="G542" s="5"/>
     </row>
-    <row r="543" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="543" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F543" s="4"/>
       <c r="G543" s="5"/>
     </row>
-    <row r="544" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="544" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F544" s="4"/>
       <c r="G544" s="5"/>
     </row>
-    <row r="545" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="545" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F545" s="4"/>
       <c r="G545" s="5"/>
     </row>
-    <row r="546" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="546" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F546" s="4"/>
       <c r="G546" s="5"/>
     </row>
-    <row r="547" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="547" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F547" s="4"/>
       <c r="G547" s="5"/>
     </row>
-    <row r="548" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="548" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F548" s="4"/>
       <c r="G548" s="5"/>
     </row>
-    <row r="549" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="549" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F549" s="4"/>
       <c r="G549" s="5"/>
     </row>
-    <row r="550" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="550" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F550" s="4"/>
       <c r="G550" s="5"/>
     </row>
-    <row r="551" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="551" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F551" s="4"/>
       <c r="G551" s="5"/>
     </row>
-    <row r="552" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="552" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F552" s="4"/>
       <c r="G552" s="5"/>
     </row>
-    <row r="553" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="553" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F553" s="4"/>
       <c r="G553" s="5"/>
     </row>
-    <row r="554" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="554" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F554" s="4"/>
       <c r="G554" s="5"/>
     </row>
-    <row r="555" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="555" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F555" s="4"/>
       <c r="G555" s="5"/>
     </row>
-    <row r="556" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="556" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F556" s="4"/>
       <c r="G556" s="5"/>
     </row>
-    <row r="557" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="557" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F557" s="4"/>
       <c r="G557" s="5"/>
     </row>
-    <row r="558" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="558" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F558" s="4"/>
       <c r="G558" s="5"/>
     </row>
-    <row r="559" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="559" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F559" s="4"/>
       <c r="G559" s="5"/>
     </row>
-    <row r="560" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="560" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F560" s="4"/>
       <c r="G560" s="5"/>
     </row>
-    <row r="561" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="561" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F561" s="4"/>
       <c r="G561" s="5"/>
     </row>
-    <row r="562" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="562" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F562" s="4"/>
       <c r="G562" s="5"/>
     </row>
-    <row r="563" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="563" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F563" s="4"/>
       <c r="G563" s="5"/>
     </row>
-    <row r="564" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="564" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F564" s="4"/>
       <c r="G564" s="5"/>
     </row>
-    <row r="565" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="565" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F565" s="4"/>
       <c r="G565" s="5"/>
     </row>
-    <row r="566" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="566" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F566" s="4"/>
       <c r="G566" s="5"/>
     </row>
-    <row r="567" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="567" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F567" s="4"/>
       <c r="G567" s="5"/>
     </row>
-    <row r="568" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="568" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F568" s="4"/>
       <c r="G568" s="5"/>
     </row>
-    <row r="569" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="569" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F569" s="4"/>
       <c r="G569" s="5"/>
     </row>
-    <row r="570" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="570" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F570" s="4"/>
       <c r="G570" s="5"/>
     </row>
-    <row r="571" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="571" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F571" s="4"/>
       <c r="G571" s="5"/>
     </row>
-    <row r="572" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="572" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F572" s="4"/>
       <c r="G572" s="5"/>
     </row>
-    <row r="573" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="573" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F573" s="4"/>
       <c r="G573" s="5"/>
     </row>
-    <row r="574" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="574" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F574" s="4"/>
       <c r="G574" s="5"/>
     </row>
-    <row r="575" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="575" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F575" s="4"/>
       <c r="G575" s="5"/>
     </row>
-    <row r="576" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="576" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F576" s="4"/>
       <c r="G576" s="5"/>
     </row>
-    <row r="577" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="577" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F577" s="4"/>
       <c r="G577" s="5"/>
     </row>
-    <row r="578" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="578" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F578" s="4"/>
       <c r="G578" s="5"/>
     </row>
-    <row r="579" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="579" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F579" s="4"/>
       <c r="G579" s="5"/>
     </row>
-    <row r="580" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="580" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F580" s="4"/>
       <c r="G580" s="5"/>
     </row>
-    <row r="581" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="581" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F581" s="4"/>
       <c r="G581" s="5"/>
     </row>
-    <row r="582" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="582" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F582" s="4"/>
       <c r="G582" s="5"/>
     </row>
-    <row r="583" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="583" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F583" s="4"/>
       <c r="G583" s="5"/>
     </row>
-    <row r="584" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="584" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F584" s="4"/>
       <c r="G584" s="5"/>
     </row>
-    <row r="585" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="585" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F585" s="4"/>
       <c r="G585" s="5"/>
     </row>
-    <row r="586" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="586" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F586" s="4"/>
       <c r="G586" s="5"/>
     </row>
-    <row r="587" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="587" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F587" s="4"/>
       <c r="G587" s="5"/>
     </row>
-    <row r="588" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="588" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F588" s="4"/>
       <c r="G588" s="5"/>
     </row>
-    <row r="589" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="589" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F589" s="4"/>
       <c r="G589" s="5"/>
     </row>
-    <row r="590" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="590" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F590" s="4"/>
       <c r="G590" s="5"/>
     </row>
-    <row r="591" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="591" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F591" s="4"/>
       <c r="G591" s="5"/>
     </row>
-    <row r="592" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="592" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F592" s="4"/>
       <c r="G592" s="5"/>
     </row>
-    <row r="593" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="593" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F593" s="4"/>
       <c r="G593" s="5"/>
     </row>
-    <row r="594" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="594" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F594" s="4"/>
       <c r="G594" s="5"/>
     </row>
-    <row r="595" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="595" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F595" s="4"/>
       <c r="G595" s="5"/>
     </row>
-    <row r="596" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="596" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F596" s="4"/>
       <c r="G596" s="5"/>
     </row>
-    <row r="597" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="597" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F597" s="4"/>
       <c r="G597" s="5"/>
     </row>
-    <row r="598" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="598" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F598" s="4"/>
       <c r="G598" s="5"/>
     </row>
-    <row r="599" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="599" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F599" s="4"/>
       <c r="G599" s="5"/>
     </row>
-    <row r="600" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="600" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F600" s="4"/>
       <c r="G600" s="5"/>
     </row>
-    <row r="601" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="601" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F601" s="4"/>
       <c r="G601" s="5"/>
     </row>
-    <row r="602" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="602" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F602" s="4"/>
       <c r="G602" s="5"/>
     </row>
-    <row r="603" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="603" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F603" s="4"/>
       <c r="G603" s="5"/>
     </row>
-    <row r="604" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="604" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F604" s="4"/>
       <c r="G604" s="5"/>
     </row>
-    <row r="605" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="605" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F605" s="4"/>
       <c r="G605" s="5"/>
     </row>
-    <row r="606" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="606" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F606" s="4"/>
       <c r="G606" s="5"/>
     </row>
-    <row r="607" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="607" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F607" s="4"/>
       <c r="G607" s="5"/>
     </row>
-    <row r="608" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="608" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F608" s="4"/>
       <c r="G608" s="5"/>
     </row>
-    <row r="609" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="609" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F609" s="4"/>
       <c r="G609" s="5"/>
     </row>
-    <row r="610" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="610" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F610" s="4"/>
       <c r="G610" s="5"/>
     </row>
-    <row r="611" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="611" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F611" s="4"/>
       <c r="G611" s="5"/>
     </row>
-    <row r="612" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="612" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F612" s="4"/>
       <c r="G612" s="5"/>
     </row>
-    <row r="613" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="613" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F613" s="4"/>
       <c r="G613" s="5"/>
     </row>
-    <row r="614" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="614" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F614" s="4"/>
       <c r="G614" s="5"/>
     </row>
-    <row r="615" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="615" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F615" s="4"/>
       <c r="G615" s="5"/>
     </row>
-    <row r="616" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="616" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F616" s="4"/>
       <c r="G616" s="5"/>
     </row>
-    <row r="617" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="617" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F617" s="4"/>
       <c r="G617" s="5"/>
     </row>
-    <row r="618" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="618" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F618" s="4"/>
       <c r="G618" s="5"/>
     </row>
-    <row r="619" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="619" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F619" s="4"/>
       <c r="G619" s="5"/>
     </row>
-    <row r="620" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="620" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F620" s="4"/>
       <c r="G620" s="5"/>
     </row>
-    <row r="621" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="621" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F621" s="4"/>
       <c r="G621" s="5"/>
     </row>
-    <row r="622" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="622" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F622" s="4"/>
       <c r="G622" s="5"/>
     </row>
-    <row r="623" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="623" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F623" s="4"/>
       <c r="G623" s="5"/>
     </row>
-    <row r="624" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="624" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F624" s="4"/>
       <c r="G624" s="5"/>
     </row>
-    <row r="625" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="625" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F625" s="4"/>
       <c r="G625" s="5"/>
     </row>
-    <row r="626" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="626" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F626" s="4"/>
       <c r="G626" s="5"/>
     </row>
-    <row r="627" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="627" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F627" s="4"/>
       <c r="G627" s="5"/>
     </row>
-    <row r="628" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="628" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F628" s="4"/>
       <c r="G628" s="5"/>
     </row>
-    <row r="629" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="629" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F629" s="4"/>
       <c r="G629" s="5"/>
     </row>
-    <row r="630" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="630" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F630" s="4"/>
       <c r="G630" s="5"/>
     </row>
-    <row r="631" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="631" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F631" s="4"/>
       <c r="G631" s="5"/>
     </row>
-    <row r="632" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="632" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F632" s="4"/>
       <c r="G632" s="5"/>
     </row>
-    <row r="633" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="633" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F633" s="4"/>
       <c r="G633" s="5"/>
     </row>
-    <row r="634" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="634" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F634" s="4"/>
       <c r="G634" s="5"/>
     </row>
-    <row r="635" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="635" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F635" s="4"/>
       <c r="G635" s="5"/>
     </row>
-    <row r="636" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="636" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F636" s="4"/>
       <c r="G636" s="5"/>
     </row>
-    <row r="637" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="637" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F637" s="4"/>
       <c r="G637" s="5"/>
     </row>
-    <row r="638" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="638" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F638" s="4"/>
       <c r="G638" s="5"/>
     </row>
-    <row r="639" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="639" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F639" s="4"/>
       <c r="G639" s="5"/>
     </row>
-    <row r="640" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="640" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F640" s="4"/>
       <c r="G640" s="5"/>
     </row>
-    <row r="641" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="641" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F641" s="4"/>
       <c r="G641" s="5"/>
     </row>
-    <row r="642" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="642" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F642" s="4"/>
       <c r="G642" s="5"/>
     </row>
-    <row r="643" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="643" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F643" s="4"/>
       <c r="G643" s="5"/>
     </row>
-    <row r="644" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="644" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F644" s="4"/>
       <c r="G644" s="5"/>
     </row>
-    <row r="645" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="645" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F645" s="4"/>
       <c r="G645" s="5"/>
     </row>
-    <row r="646" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="646" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F646" s="4"/>
       <c r="G646" s="5"/>
     </row>
-    <row r="647" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="647" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F647" s="4"/>
       <c r="G647" s="5"/>
     </row>
-    <row r="648" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="648" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F648" s="4"/>
       <c r="G648" s="5"/>
     </row>
-    <row r="649" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="649" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F649" s="4"/>
       <c r="G649" s="5"/>
     </row>
-    <row r="650" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="650" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F650" s="4"/>
       <c r="G650" s="5"/>
     </row>
-    <row r="651" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="651" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F651" s="4"/>
       <c r="G651" s="5"/>
     </row>
-    <row r="652" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="652" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F652" s="4"/>
       <c r="G652" s="5"/>
     </row>
-    <row r="653" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="653" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F653" s="4"/>
       <c r="G653" s="5"/>
     </row>
-    <row r="654" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="654" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F654" s="4"/>
       <c r="G654" s="5"/>
     </row>
-    <row r="655" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="655" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F655" s="4"/>
       <c r="G655" s="5"/>
     </row>
-    <row r="656" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="656" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F656" s="4"/>
       <c r="G656" s="5"/>
     </row>
-    <row r="657" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="657" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F657" s="4"/>
       <c r="G657" s="5"/>
     </row>
-    <row r="658" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="658" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F658" s="4"/>
       <c r="G658" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879E7154-DDA4-43DA-89F0-1E0155F85108}">
+  <dimension ref="D5:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(data[Amount])</f>
+        <v>4136.2299999999996</v>
+      </c>
+      <c r="F6">
+        <f>AVERAGE(data[Units])</f>
+        <v>152.19999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <f>MEDIAN(data[Amount])</f>
+        <v>3437</v>
+      </c>
+      <c r="F7">
+        <f>MEDIAN(data[Units])</f>
+        <v>124.5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8">
+        <f>MIN(data[Amount])</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>MIN(data[Units])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <f>MAX(data[Amount])</f>
+        <v>16184</v>
+      </c>
+      <c r="F9">
+        <f>MAX(data[Units])</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10">
+        <f>E9-E8</f>
+        <v>16184</v>
+      </c>
+      <c r="F10">
+        <f>F9-F8</f>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>